<commit_message>
03042023 - Getting Tweets per Team MOS & EOS
</commit_message>
<xml_diff>
--- a/Dissertation 2023 - Bachelor Degree/Team Sheet.xlsx
+++ b/Dissertation 2023 - Bachelor Degree/Team Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e55a912db83fd400/Desktop/DissertationRepository2023/Dissertation 2023 - Bachelor Degree/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D8C533A0-1782-42D2-B1BC-0140A828B64C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="8_{D8C533A0-1782-42D2-B1BC-0140A828B64C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{908BF299-BA76-4E66-8F55-D2561C11E50D}"/>
   <bookViews>
-    <workbookView xWindow="3585" yWindow="2895" windowWidth="22980" windowHeight="12195" activeTab="3" xr2:uid="{2ED4C26E-24C0-45A0-9093-857D516C9F7A}"/>
+    <workbookView xWindow="-23565" yWindow="2175" windowWidth="17280" windowHeight="8880" firstSheet="1" activeTab="2" xr2:uid="{2ED4C26E-24C0-45A0-9093-857D516C9F7A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="49">
   <si>
     <t>West Ham United</t>
   </si>
@@ -177,6 +177,15 @@
   </si>
   <si>
     <t>#ncfc</t>
+  </si>
+  <si>
+    <t>#mcfc</t>
+  </si>
+  <si>
+    <t>#saintsfc</t>
+  </si>
+  <si>
+    <t>#thfc</t>
   </si>
 </sst>
 </file>
@@ -192,7 +201,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -208,6 +217,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -230,7 +245,7 @@
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -246,6 +261,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -548,7 +567,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I20" sqref="H1:I20"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -716,10 +735,10 @@
       <c r="D8" t="s">
         <v>32</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8">
         <v>8</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="I8" t="s">
         <v>14</v>
       </c>
     </row>
@@ -744,10 +763,10 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H10" s="5">
+      <c r="H10">
         <v>10</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="I10" t="s">
         <v>16</v>
       </c>
     </row>
@@ -760,10 +779,10 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H12" s="5">
+      <c r="H12">
         <v>12</v>
       </c>
-      <c r="I12" s="5" t="s">
+      <c r="I12" t="s">
         <v>20</v>
       </c>
     </row>
@@ -784,18 +803,18 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H15" s="5">
+      <c r="H15">
         <v>15</v>
       </c>
-      <c r="I15" s="5" t="s">
+      <c r="I15" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H16" s="5">
+      <c r="H16">
         <v>16</v>
       </c>
-      <c r="I16" s="5" t="s">
+      <c r="I16" t="s">
         <v>24</v>
       </c>
     </row>
@@ -808,10 +827,10 @@
       </c>
     </row>
     <row r="18" spans="8:10" x14ac:dyDescent="0.3">
-      <c r="H18" s="5">
+      <c r="H18">
         <v>18</v>
       </c>
-      <c r="I18" s="5" t="s">
+      <c r="I18" t="s">
         <v>25</v>
       </c>
       <c r="J18" t="s">
@@ -819,10 +838,10 @@
       </c>
     </row>
     <row r="19" spans="8:10" x14ac:dyDescent="0.3">
-      <c r="H19" s="5">
+      <c r="H19">
         <v>19</v>
       </c>
-      <c r="I19" s="5" t="s">
+      <c r="I19" t="s">
         <v>27</v>
       </c>
       <c r="J19" t="s">
@@ -830,10 +849,10 @@
       </c>
     </row>
     <row r="20" spans="8:10" x14ac:dyDescent="0.3">
-      <c r="H20" s="5">
+      <c r="H20">
         <v>20</v>
       </c>
-      <c r="I20" s="5" t="s">
+      <c r="I20" t="s">
         <v>28</v>
       </c>
       <c r="J20" t="s">
@@ -859,10 +878,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="5">
+      <c r="A1">
         <v>1</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" t="s">
         <v>8</v>
       </c>
       <c r="C1" t="s">
@@ -870,10 +889,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="5">
+      <c r="A2">
         <v>2</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" t="s">
         <v>9</v>
       </c>
       <c r="C2" t="s">
@@ -881,10 +900,10 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="5">
+      <c r="A3">
         <v>3</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" t="s">
         <v>5</v>
       </c>
       <c r="C3" t="s">
@@ -892,10 +911,10 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="5">
+      <c r="A4">
         <v>4</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" t="s">
         <v>10</v>
       </c>
       <c r="C4" t="s">
@@ -903,10 +922,10 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="5">
+      <c r="A5">
         <v>5</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" t="s">
         <v>11</v>
       </c>
       <c r="C5" t="s">
@@ -925,10 +944,10 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="5">
+      <c r="A7">
         <v>7</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" t="s">
         <v>13</v>
       </c>
       <c r="C7" t="s">
@@ -936,10 +955,10 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="5">
+      <c r="A8">
         <v>8</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" t="s">
         <v>14</v>
       </c>
       <c r="C8" t="s">
@@ -947,10 +966,10 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="5">
+      <c r="A9">
         <v>9</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" t="s">
         <v>15</v>
       </c>
       <c r="C9" t="s">
@@ -958,10 +977,10 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="5">
+      <c r="A10">
         <v>10</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" t="s">
         <v>16</v>
       </c>
       <c r="C10" t="s">
@@ -969,10 +988,10 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="5">
+      <c r="A11">
         <v>11</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" t="s">
         <v>17</v>
       </c>
       <c r="C11" t="s">
@@ -980,10 +999,10 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="5">
+      <c r="A12">
         <v>12</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" t="s">
         <v>20</v>
       </c>
       <c r="C12" t="s">
@@ -991,10 +1010,10 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="5">
+      <c r="A13">
         <v>13</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" t="s">
         <v>21</v>
       </c>
       <c r="C13" t="s">
@@ -1002,10 +1021,10 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="5">
+      <c r="A14">
         <v>14</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" t="s">
         <v>22</v>
       </c>
       <c r="C14" t="s">
@@ -1013,10 +1032,10 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="5">
+      <c r="A15">
         <v>15</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" t="s">
         <v>23</v>
       </c>
       <c r="C15" t="s">
@@ -1024,10 +1043,10 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="5">
+      <c r="A16">
         <v>16</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" t="s">
         <v>24</v>
       </c>
       <c r="C16" t="s">
@@ -1035,10 +1054,10 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="5">
+      <c r="A17">
         <v>17</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" t="s">
         <v>3</v>
       </c>
       <c r="C17" t="s">
@@ -1046,10 +1065,10 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="5">
+      <c r="A18">
         <v>18</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" t="s">
         <v>25</v>
       </c>
       <c r="C18" t="s">
@@ -1057,10 +1076,10 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="5">
+      <c r="A19">
         <v>19</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" t="s">
         <v>27</v>
       </c>
       <c r="C19" t="s">
@@ -1068,10 +1087,10 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="5">
+      <c r="A20">
         <v>20</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" t="s">
         <v>28</v>
       </c>
       <c r="C20" t="s">
@@ -1087,31 +1106,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52F357D5-1E71-4112-843E-5FB5870196DD}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="5">
+      <c r="A1" s="4">
         <v>1</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="5">
+      <c r="A2" s="4">
         <v>2</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="4" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1127,35 +1146,35 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="5">
+      <c r="A4" s="4">
         <v>4</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
-        <v>37</v>
+      <c r="C4" s="4" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="5">
+      <c r="A5" s="4">
         <v>5</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
-        <v>29</v>
+      <c r="C5" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
+      <c r="A6" s="4">
         <v>6</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="4" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1166,7 +1185,7 @@
       <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="5" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1177,7 +1196,7 @@
       <c r="B8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="5" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1188,7 +1207,7 @@
       <c r="B9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="5" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1199,37 +1218,37 @@
       <c r="B10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="5">
+      <c r="A11" s="4">
         <v>11</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="5">
+      <c r="A12" s="4">
         <v>12</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="4" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="5">
+      <c r="A13">
         <v>13</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" t="s">
         <v>21</v>
       </c>
       <c r="C13" t="s">
@@ -1237,10 +1256,10 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="5">
+      <c r="A14">
         <v>14</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" t="s">
         <v>22</v>
       </c>
       <c r="C14" t="s">
@@ -1248,10 +1267,10 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="5">
+      <c r="A15">
         <v>15</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" t="s">
         <v>23</v>
       </c>
       <c r="C15" t="s">
@@ -1259,10 +1278,10 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="5">
+      <c r="A16">
         <v>16</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" t="s">
         <v>24</v>
       </c>
       <c r="C16" t="s">
@@ -1270,10 +1289,10 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="5">
+      <c r="A17">
         <v>17</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" t="s">
         <v>3</v>
       </c>
       <c r="C17" t="s">
@@ -1281,10 +1300,10 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="5">
+      <c r="A18">
         <v>18</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" t="s">
         <v>25</v>
       </c>
       <c r="C18" t="s">
@@ -1292,10 +1311,10 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="5">
+      <c r="A19">
         <v>19</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" t="s">
         <v>27</v>
       </c>
       <c r="C19" t="s">
@@ -1303,10 +1322,10 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="5">
+      <c r="A20">
         <v>20</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" t="s">
         <v>28</v>
       </c>
       <c r="C20" t="s">
@@ -1322,8 +1341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E724BFA1-1C95-4746-A80E-97B36BC29E40}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1340,7 +1359,7 @@
         <v>8</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1355,13 +1374,13 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="5">
+      <c r="A3" s="4">
         <v>3</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1373,7 +1392,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1384,17 +1403,17 @@
         <v>11</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
+      <c r="A6" s="4">
         <v>6</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="4" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1494,7 +1513,7 @@
         <v>23</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Methodology Draft 2 without Prototype Pipeline
</commit_message>
<xml_diff>
--- a/Dissertation 2023 - Bachelor Degree/Team Sheet.xlsx
+++ b/Dissertation 2023 - Bachelor Degree/Team Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e55a912db83fd400/Desktop/DissertationRepository2023/Dissertation 2023 - Bachelor Degree/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="8_{D8C533A0-1782-42D2-B1BC-0140A828B64C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{908BF299-BA76-4E66-8F55-D2561C11E50D}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="8_{D8C533A0-1782-42D2-B1BC-0140A828B64C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{70A75E9C-9CB1-48D5-87C0-2A282FBF45D7}"/>
   <bookViews>
-    <workbookView xWindow="-23565" yWindow="2175" windowWidth="17280" windowHeight="8880" firstSheet="1" activeTab="2" xr2:uid="{2ED4C26E-24C0-45A0-9093-857D516C9F7A}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8880" firstSheet="1" activeTab="2" xr2:uid="{2ED4C26E-24C0-45A0-9093-857D516C9F7A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1106,8 +1106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52F357D5-1E71-4112-843E-5FB5870196DD}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1256,13 +1256,13 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14">
+      <c r="A14" s="4">
         <v>14</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="4" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1278,13 +1278,13 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16">
+      <c r="A16" s="4">
         <v>16</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="4" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Stopwords -> Hybrid & NB
Hybrid LSTM+CNN with Stopwords, Modified Naive Bayes to use stop words, less accuracy
</commit_message>
<xml_diff>
--- a/Dissertation 2023 - Bachelor Degree/Team Sheet.xlsx
+++ b/Dissertation 2023 - Bachelor Degree/Team Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e55a912db83fd400/Desktop/DissertationRepository2023/Dissertation 2023 - Bachelor Degree/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="46" documentId="8_{D8C533A0-1782-42D2-B1BC-0140A828B64C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{70A75E9C-9CB1-48D5-87C0-2A282FBF45D7}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="8_{D8C533A0-1782-42D2-B1BC-0140A828B64C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7C2BACBD-3122-48E7-8B4E-3F5227758713}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8880" firstSheet="1" activeTab="2" xr2:uid="{2ED4C26E-24C0-45A0-9093-857D516C9F7A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="2" xr2:uid="{2ED4C26E-24C0-45A0-9093-857D516C9F7A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1106,8 +1106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52F357D5-1E71-4112-843E-5FB5870196DD}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1289,13 +1289,13 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17">
+      <c r="A17" s="4">
         <v>17</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="4" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1322,13 +1322,13 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20">
+      <c r="A20" s="4">
         <v>20</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="4" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Stop Words Implementation - Different types of Models. Continuation of Tweets Extracting, Logbook and Updated RQs
</commit_message>
<xml_diff>
--- a/Dissertation 2023 - Bachelor Degree/Team Sheet.xlsx
+++ b/Dissertation 2023 - Bachelor Degree/Team Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e55a912db83fd400/Desktop/DissertationRepository2023/Dissertation 2023 - Bachelor Degree/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="8_{D8C533A0-1782-42D2-B1BC-0140A828B64C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7C2BACBD-3122-48E7-8B4E-3F5227758713}"/>
+  <xr:revisionPtr revIDLastSave="64" documentId="8_{D8C533A0-1782-42D2-B1BC-0140A828B64C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72E8C9A7-7AF4-4FE4-A6F9-8DFBA71DFD62}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="2" xr2:uid="{2ED4C26E-24C0-45A0-9093-857D516C9F7A}"/>
+    <workbookView minimized="1" xWindow="56595" yWindow="570" windowWidth="24255" windowHeight="15285" firstSheet="1" activeTab="1" xr2:uid="{2ED4C26E-24C0-45A0-9093-857D516C9F7A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -222,7 +222,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -868,13 +868,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{755FA705-5A57-405A-8339-221E31590121}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -933,10 +934,10 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="4">
+      <c r="A6">
         <v>6</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" t="s">
         <v>12</v>
       </c>
       <c r="C6" t="s">
@@ -1032,13 +1033,13 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15">
+      <c r="A15" s="5">
         <v>15</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="5" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1106,11 +1107,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52F357D5-1E71-4112-843E-5FB5870196DD}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="4">
@@ -1179,46 +1184,46 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="5">
+      <c r="A7" s="4">
         <v>7</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="5">
+      <c r="A8" s="4">
         <v>8</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="5">
+      <c r="A9" s="4">
         <v>9</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="5">
+      <c r="A10" s="4">
         <v>10</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1245,13 +1250,13 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13">
+      <c r="A13" s="4">
         <v>13</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="4" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1267,13 +1272,13 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15">
+      <c r="A15" s="4">
         <v>15</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="4" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1300,24 +1305,24 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18">
+      <c r="A18" s="4">
         <v>18</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19">
+      <c r="A19" s="4">
         <v>19</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="4" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>